<commit_message>
Fully implemented all data for the today query
</commit_message>
<xml_diff>
--- a/Services/StateOfTexas/Data/CumulativeTestsOverTimeByCounty.xlsx
+++ b/Services/StateOfTexas/Data/CumulativeTestsOverTimeByCounty.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\CMartStudios\collincountycoviddashboard\CovidActNowAPIClient\StateOfTexas\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Development\CMartStudios\collincountycoviddashboard\Services\StateOfTexas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C58ED7D1-F707-4883-A677-B3211D700D9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA398C12-2B56-4F8F-970F-8E70002A7370}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{09D2CA0E-9107-4430-A0C0-2B01BAE5A0A0}"/>
+    <workbookView xWindow="57480" yWindow="2205" windowWidth="24240" windowHeight="13140" xr2:uid="{09D2CA0E-9107-4430-A0C0-2B01BAE5A0A0}"/>
   </bookViews>
   <sheets>
     <sheet name="Total Tests" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -235,6 +235,12 @@
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -547,7 +553,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="80">
+  <cellStyleXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -628,8 +634,10 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -640,8 +648,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="80">
+  <cellStyles count="82">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
@@ -684,6 +693,8 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="76" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
     <cellStyle name="Normal 11" xfId="79" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 11 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="Normal 12" xfId="81" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{F5C747AA-F0F3-427C-9470-C9FB9C452FE3}"/>
     <cellStyle name="Normal 2 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
     <cellStyle name="Normal 2 2 2" xfId="52" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
@@ -1033,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46C8CE8-D917-42CC-8F81-F51BED46A69F}">
-  <dimension ref="A1:BV257"/>
+  <dimension ref="A1:CD257"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1063,9 +1074,16 @@
     <col min="71" max="71" width="10.5" style="5" customWidth="1"/>
     <col min="72" max="72" width="10.19921875" style="5" customWidth="1"/>
     <col min="73" max="73" width="10.69921875" style="5" customWidth="1"/>
+    <col min="74" max="74" width="10.59765625" customWidth="1"/>
+    <col min="75" max="75" width="11" customWidth="1"/>
+    <col min="76" max="78" width="11" style="6" customWidth="1"/>
+    <col min="79" max="79" width="10.09765625" customWidth="1"/>
+    <col min="80" max="80" width="10.296875" style="6" customWidth="1"/>
+    <col min="81" max="81" width="10.296875" customWidth="1"/>
+    <col min="82" max="82" width="10.796875" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1288,8 +1306,32 @@
       <c r="BV1" s="3">
         <v>44159</v>
       </c>
-    </row>
-    <row r="2" spans="1:74" x14ac:dyDescent="0.2">
+      <c r="BW1" s="3">
+        <v>44160</v>
+      </c>
+      <c r="BX1" s="3">
+        <v>44161</v>
+      </c>
+      <c r="BY1" s="3">
+        <v>44162</v>
+      </c>
+      <c r="BZ1" s="3">
+        <v>44163</v>
+      </c>
+      <c r="CA1" s="3">
+        <v>44164</v>
+      </c>
+      <c r="CB1" s="3">
+        <v>44165</v>
+      </c>
+      <c r="CC1" s="3">
+        <v>44166</v>
+      </c>
+      <c r="CD1" s="3">
+        <v>44167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:82" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1512,8 +1554,32 @@
       <c r="BV2" s="2">
         <v>461310</v>
       </c>
-    </row>
-    <row r="3" spans="1:74" x14ac:dyDescent="0.2">
+      <c r="BW2" s="2">
+        <v>464746</v>
+      </c>
+      <c r="BX2" s="2">
+        <v>469728</v>
+      </c>
+      <c r="BY2" s="2">
+        <v>475706</v>
+      </c>
+      <c r="BZ2" s="2">
+        <v>478051</v>
+      </c>
+      <c r="CA2" s="2">
+        <v>480689</v>
+      </c>
+      <c r="CB2" s="2">
+        <v>486111</v>
+      </c>
+      <c r="CC2" s="2">
+        <v>489592</v>
+      </c>
+      <c r="CD2" s="2">
+        <v>493103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:82" x14ac:dyDescent="0.2">
       <c r="J3" t="s">
         <v>2</v>
       </c>
@@ -1540,7 +1606,7 @@
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
     </row>
-    <row r="4" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1548,7 +1614,7 @@
       <c r="S4" s="2"/>
       <c r="T4" s="2"/>
     </row>
-    <row r="5" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -1556,7 +1622,7 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
     </row>
-    <row r="6" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -1564,7 +1630,7 @@
       <c r="S6" s="2"/>
       <c r="T6" s="2"/>
     </row>
-    <row r="7" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M7" s="2"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -1572,7 +1638,7 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
     </row>
-    <row r="8" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -1580,7 +1646,7 @@
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
     </row>
-    <row r="9" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -1588,7 +1654,7 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
     </row>
-    <row r="10" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -1596,7 +1662,7 @@
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
     </row>
-    <row r="11" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -1604,7 +1670,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -1612,7 +1678,7 @@
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
     </row>
-    <row r="13" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -1620,7 +1686,7 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
     </row>
-    <row r="14" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -1628,7 +1694,7 @@
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
     </row>
-    <row r="15" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -1636,7 +1702,7 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:74" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:82" x14ac:dyDescent="0.2">
       <c r="M16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>

</xml_diff>

<commit_message>
Data Update 12/20/2020 Set new cases header as "New Confirmed Cases"
</commit_message>
<xml_diff>
--- a/Services/StateOfTexas/Data/CumulativeTestsOverTimeByCounty.xlsx
+++ b/Services/StateOfTexas/Data/CumulativeTestsOverTimeByCounty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\CHS-AAU\Epi\Covid\For Ektron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{34345E81-E8AD-4E98-8AC3-2BC2D8420773}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E405AA0-4FAE-413C-8915-835BF62D1BAF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11900" xr2:uid="{09D2CA0E-9107-4430-A0C0-2B01BAE5A0A0}"/>
   </bookViews>
@@ -1834,7 +1834,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46C8CE8-D917-42CC-8F81-F51BED46A69F}">
-  <dimension ref="A1:CT513"/>
+  <dimension ref="A1:CU513"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1869,15 +1869,15 @@
     <col min="80" max="80" width="10.265625" style="7" customWidth="1"/>
     <col min="81" max="81" width="10.33203125" customWidth="1"/>
     <col min="82" max="90" width="10.796875" style="7" customWidth="1"/>
-    <col min="91" max="98" width="9.86328125" style="7" bestFit="1" customWidth="1"/>
+    <col min="91" max="99" width="9.86328125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="2" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>255</v>
       </c>
@@ -2172,8 +2172,11 @@
       <c r="CT2" s="4">
         <v>44183</v>
       </c>
+      <c r="CU2" s="4">
+        <v>44184</v>
+      </c>
     </row>
-    <row r="3" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2468,8 +2471,11 @@
       <c r="CT3" s="2">
         <v>41011</v>
       </c>
+      <c r="CU3" s="2">
+        <v>41302</v>
+      </c>
     </row>
-    <row r="4" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -2764,8 +2770,11 @@
       <c r="CT4" s="2">
         <v>4576</v>
       </c>
+      <c r="CU4" s="2">
+        <v>4594</v>
+      </c>
     </row>
-    <row r="5" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -3060,8 +3069,11 @@
       <c r="CT5" s="2">
         <v>42085</v>
       </c>
+      <c r="CU5" s="2">
+        <v>42779</v>
+      </c>
     </row>
-    <row r="6" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -3356,8 +3368,11 @@
       <c r="CT6" s="2">
         <v>7615</v>
       </c>
+      <c r="CU6" s="2">
+        <v>7710</v>
+      </c>
     </row>
-    <row r="7" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -3652,8 +3667,11 @@
       <c r="CT7" s="2">
         <v>2058</v>
       </c>
+      <c r="CU7" s="2">
+        <v>2084</v>
+      </c>
     </row>
-    <row r="8" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -3948,8 +3966,11 @@
       <c r="CT8" s="2">
         <v>587</v>
       </c>
+      <c r="CU8" s="2">
+        <v>594</v>
+      </c>
     </row>
-    <row r="9" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -4244,8 +4265,11 @@
       <c r="CT9" s="2">
         <v>22205</v>
       </c>
+      <c r="CU9" s="2">
+        <v>22410</v>
+      </c>
     </row>
-    <row r="10" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -4540,8 +4564,11 @@
       <c r="CT10" s="2">
         <v>11053</v>
       </c>
+      <c r="CU10" s="2">
+        <v>11186</v>
+      </c>
     </row>
-    <row r="11" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -4836,8 +4863,11 @@
       <c r="CT11" s="2">
         <v>1764</v>
       </c>
+      <c r="CU11" s="2">
+        <v>1769</v>
+      </c>
     </row>
-    <row r="12" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -5132,8 +5162,11 @@
       <c r="CT12" s="2">
         <v>5946</v>
       </c>
+      <c r="CU12" s="2">
+        <v>6007</v>
+      </c>
     </row>
-    <row r="13" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -5428,8 +5461,11 @@
       <c r="CT13" s="2">
         <v>33145</v>
       </c>
+      <c r="CU13" s="2">
+        <v>33609</v>
+      </c>
     </row>
-    <row r="14" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -5724,8 +5760,11 @@
       <c r="CT14" s="2">
         <v>1264</v>
       </c>
+      <c r="CU14" s="2">
+        <v>1268</v>
+      </c>
     </row>
-    <row r="15" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -6020,8 +6059,11 @@
       <c r="CT15" s="2">
         <v>27640</v>
       </c>
+      <c r="CU15" s="2">
+        <v>27797</v>
+      </c>
     </row>
-    <row r="16" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -6316,8 +6358,11 @@
       <c r="CT16" s="2">
         <v>157215</v>
       </c>
+      <c r="CU16" s="2">
+        <v>159345</v>
+      </c>
     </row>
-    <row r="17" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -6612,8 +6657,11 @@
       <c r="CT17" s="2">
         <v>924756</v>
       </c>
+      <c r="CU17" s="2">
+        <v>933282</v>
+      </c>
     </row>
-    <row r="18" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -6908,8 +6956,11 @@
       <c r="CT18" s="2">
         <v>3594</v>
       </c>
+      <c r="CU18" s="2">
+        <v>3648</v>
+      </c>
     </row>
-    <row r="19" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -7204,8 +7255,11 @@
       <c r="CT19" s="2">
         <v>92</v>
       </c>
+      <c r="CU19" s="2">
+        <v>92</v>
+      </c>
     </row>
-    <row r="20" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -7500,8 +7554,11 @@
       <c r="CT20" s="2">
         <v>9370</v>
       </c>
+      <c r="CU20" s="2">
+        <v>9456</v>
+      </c>
     </row>
-    <row r="21" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -7796,8 +7853,11 @@
       <c r="CT21" s="2">
         <v>52889</v>
       </c>
+      <c r="CU21" s="2">
+        <v>53280</v>
+      </c>
     </row>
-    <row r="22" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -8092,8 +8152,11 @@
       <c r="CT22" s="2">
         <v>204698</v>
       </c>
+      <c r="CU22" s="2">
+        <v>206195</v>
+      </c>
     </row>
-    <row r="23" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -8388,8 +8451,11 @@
       <c r="CT23" s="2">
         <v>142756</v>
       </c>
+      <c r="CU23" s="2">
+        <v>145159</v>
+      </c>
     </row>
-    <row r="24" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -8684,8 +8750,11 @@
       <c r="CT24" s="2">
         <v>7373</v>
       </c>
+      <c r="CU24" s="2">
+        <v>7443</v>
+      </c>
     </row>
-    <row r="25" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -8980,8 +9049,11 @@
       <c r="CT25" s="2">
         <v>474</v>
       </c>
+      <c r="CU25" s="2">
+        <v>474</v>
+      </c>
     </row>
-    <row r="26" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -9276,8 +9348,11 @@
       <c r="CT26" s="2">
         <v>9546</v>
       </c>
+      <c r="CU26" s="2">
+        <v>9941</v>
+      </c>
     </row>
-    <row r="27" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -9572,8 +9647,11 @@
       <c r="CT27" s="2">
         <v>18951</v>
       </c>
+      <c r="CU27" s="2">
+        <v>19033</v>
+      </c>
     </row>
-    <row r="28" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -9868,8 +9946,11 @@
       <c r="CT28" s="2">
         <v>8380</v>
       </c>
+      <c r="CU28" s="2">
+        <v>8559</v>
+      </c>
     </row>
-    <row r="29" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -10164,8 +10245,11 @@
       <c r="CT29" s="2">
         <v>20487</v>
       </c>
+      <c r="CU29" s="2">
+        <v>20802</v>
+      </c>
     </row>
-    <row r="30" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -10460,8 +10544,11 @@
       <c r="CT30" s="2">
         <v>18960</v>
       </c>
+      <c r="CU30" s="2">
+        <v>19187</v>
+      </c>
     </row>
-    <row r="31" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -10756,8 +10843,11 @@
       <c r="CT31" s="2">
         <v>9858</v>
       </c>
+      <c r="CU31" s="2">
+        <v>9899</v>
+      </c>
     </row>
-    <row r="32" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -11052,8 +11142,11 @@
       <c r="CT32" s="2">
         <v>5518</v>
       </c>
+      <c r="CU32" s="2">
+        <v>5584</v>
+      </c>
     </row>
-    <row r="33" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -11348,8 +11441,11 @@
       <c r="CT33" s="2">
         <v>174199</v>
       </c>
+      <c r="CU33" s="2">
+        <v>175597</v>
+      </c>
     </row>
-    <row r="34" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -11644,8 +11740,11 @@
       <c r="CT34" s="2">
         <v>3911</v>
       </c>
+      <c r="CU34" s="2">
+        <v>3956</v>
+      </c>
     </row>
-    <row r="35" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -11940,8 +12039,11 @@
       <c r="CT35" s="2">
         <v>1655</v>
       </c>
+      <c r="CU35" s="2">
+        <v>1659</v>
+      </c>
     </row>
-    <row r="36" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -12236,8 +12338,11 @@
       <c r="CT36" s="2">
         <v>11772</v>
       </c>
+      <c r="CU36" s="2">
+        <v>11864</v>
+      </c>
     </row>
-    <row r="37" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -12532,8 +12637,11 @@
       <c r="CT37" s="2">
         <v>3980</v>
       </c>
+      <c r="CU37" s="2">
+        <v>3997</v>
+      </c>
     </row>
-    <row r="38" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -12828,8 +12936,11 @@
       <c r="CT38" s="2">
         <v>6243</v>
       </c>
+      <c r="CU38" s="2">
+        <v>6276</v>
+      </c>
     </row>
-    <row r="39" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -13124,8 +13235,11 @@
       <c r="CT39" s="2">
         <v>17337</v>
       </c>
+      <c r="CU39" s="2">
+        <v>17471</v>
+      </c>
     </row>
-    <row r="40" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -13420,8 +13534,11 @@
       <c r="CT40" s="2">
         <v>4476</v>
       </c>
+      <c r="CU40" s="2">
+        <v>4479</v>
+      </c>
     </row>
-    <row r="41" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -13716,8 +13833,11 @@
       <c r="CT41" s="2">
         <v>2894</v>
       </c>
+      <c r="CU41" s="2">
+        <v>2924</v>
+      </c>
     </row>
-    <row r="42" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -14012,8 +14132,11 @@
       <c r="CT42" s="2">
         <v>750</v>
       </c>
+      <c r="CU42" s="2">
+        <v>753</v>
+      </c>
     </row>
-    <row r="43" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -14308,8 +14431,11 @@
       <c r="CT43" s="2">
         <v>2355</v>
       </c>
+      <c r="CU43" s="2">
+        <v>2361</v>
+      </c>
     </row>
-    <row r="44" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -14604,8 +14730,11 @@
       <c r="CT44" s="2">
         <v>2903</v>
       </c>
+      <c r="CU44" s="2">
+        <v>2919</v>
+      </c>
     </row>
-    <row r="45" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -14900,8 +15029,11 @@
       <c r="CT45" s="2">
         <v>569034</v>
       </c>
+      <c r="CU45" s="2">
+        <v>573529</v>
+      </c>
     </row>
-    <row r="46" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -15196,8 +15328,11 @@
       <c r="CT46" s="2">
         <v>1351</v>
       </c>
+      <c r="CU46" s="2">
+        <v>1351</v>
+      </c>
     </row>
-    <row r="47" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -15492,8 +15627,11 @@
       <c r="CT47" s="2">
         <v>9725</v>
       </c>
+      <c r="CU47" s="2">
+        <v>9788</v>
+      </c>
     </row>
-    <row r="48" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -15788,8 +15926,11 @@
       <c r="CT48" s="2">
         <v>61846</v>
       </c>
+      <c r="CU48" s="2">
+        <v>62815</v>
+      </c>
     </row>
-    <row r="49" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -16084,8 +16225,11 @@
       <c r="CT49" s="2">
         <v>6262</v>
       </c>
+      <c r="CU49" s="2">
+        <v>6322</v>
+      </c>
     </row>
-    <row r="50" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -16380,8 +16524,11 @@
       <c r="CT50" s="2">
         <v>1762</v>
       </c>
+      <c r="CU50" s="2">
+        <v>1764</v>
+      </c>
     </row>
-    <row r="51" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -16676,8 +16823,11 @@
       <c r="CT51" s="2">
         <v>17470</v>
       </c>
+      <c r="CU51" s="2">
+        <v>17628</v>
+      </c>
     </row>
-    <row r="52" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -16972,8 +17122,11 @@
       <c r="CT52" s="2">
         <v>60387</v>
       </c>
+      <c r="CU52" s="2">
+        <v>60617</v>
+      </c>
     </row>
-    <row r="53" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -17268,8 +17421,11 @@
       <c r="CT53" s="2">
         <v>895</v>
       </c>
+      <c r="CU53" s="2">
+        <v>895</v>
+      </c>
     </row>
-    <row r="54" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -17564,8 +17720,11 @@
       <c r="CT54" s="2">
         <v>3282</v>
       </c>
+      <c r="CU54" s="2">
+        <v>3377</v>
+      </c>
     </row>
-    <row r="55" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -17860,8 +18019,11 @@
       <c r="CT55" s="2">
         <v>1853</v>
       </c>
+      <c r="CU55" s="2">
+        <v>1856</v>
+      </c>
     </row>
-    <row r="56" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -18156,8 +18318,11 @@
       <c r="CT56" s="2">
         <v>2781</v>
       </c>
+      <c r="CU56" s="2">
+        <v>2796</v>
+      </c>
     </row>
-    <row r="57" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -18452,8 +18617,11 @@
       <c r="CT57" s="2">
         <v>1567</v>
       </c>
+      <c r="CU57" s="2">
+        <v>1629</v>
+      </c>
     </row>
-    <row r="58" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -18748,8 +18916,11 @@
       <c r="CT58" s="2">
         <v>1397</v>
       </c>
+      <c r="CU58" s="2">
+        <v>1402</v>
+      </c>
     </row>
-    <row r="59" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -19044,8 +19215,11 @@
       <c r="CT59" s="2">
         <v>1477219</v>
       </c>
+      <c r="CU59" s="2">
+        <v>1486912</v>
+      </c>
     </row>
-    <row r="60" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -19340,8 +19514,11 @@
       <c r="CT60" s="2">
         <v>6763</v>
       </c>
+      <c r="CU60" s="2">
+        <v>6794</v>
+      </c>
     </row>
-    <row r="61" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -19636,8 +19813,11 @@
       <c r="CT61" s="2">
         <v>6926</v>
       </c>
+      <c r="CU61" s="2">
+        <v>6956</v>
+      </c>
     </row>
-    <row r="62" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -19932,8 +20112,11 @@
       <c r="CT62" s="2">
         <v>4759</v>
       </c>
+      <c r="CU62" s="2">
+        <v>4767</v>
+      </c>
     </row>
-    <row r="63" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -20228,8 +20411,11 @@
       <c r="CT63" s="2">
         <v>1738</v>
       </c>
+      <c r="CU63" s="2">
+        <v>1755</v>
+      </c>
     </row>
-    <row r="64" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -20524,8 +20710,11 @@
       <c r="CT64" s="2">
         <v>353560</v>
       </c>
+      <c r="CU64" s="2">
+        <v>356971</v>
+      </c>
     </row>
-    <row r="65" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -20820,8 +21009,11 @@
       <c r="CT65" s="2">
         <v>537</v>
       </c>
+      <c r="CU65" s="2">
+        <v>538</v>
+      </c>
     </row>
-    <row r="66" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -21116,8 +21308,11 @@
       <c r="CT66" s="2">
         <v>4657</v>
       </c>
+      <c r="CU66" s="2">
+        <v>4717</v>
+      </c>
     </row>
-    <row r="67" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -21412,8 +21607,11 @@
       <c r="CT67" s="2">
         <v>1454</v>
       </c>
+      <c r="CU67" s="2">
+        <v>1457</v>
+      </c>
     </row>
-    <row r="68" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -21708,8 +21906,11 @@
       <c r="CT68" s="2">
         <v>12261</v>
       </c>
+      <c r="CU68" s="2">
+        <v>12391</v>
+      </c>
     </row>
-    <row r="69" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -22004,8 +22205,11 @@
       <c r="CT69" s="2">
         <v>4940</v>
       </c>
+      <c r="CU69" s="2">
+        <v>4968</v>
+      </c>
     </row>
-    <row r="70" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -22300,8 +22504,11 @@
       <c r="CT70" s="2">
         <v>51742</v>
       </c>
+      <c r="CU70" s="2">
+        <v>52206</v>
+      </c>
     </row>
-    <row r="71" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -22596,8 +22803,11 @@
       <c r="CT71" s="2">
         <v>1032</v>
       </c>
+      <c r="CU71" s="2">
+        <v>1035</v>
+      </c>
     </row>
-    <row r="72" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -22892,8 +23102,11 @@
       <c r="CT72" s="2">
         <v>602393</v>
       </c>
+      <c r="CU72" s="2">
+        <v>605274</v>
+      </c>
     </row>
-    <row r="73" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -23188,8 +23401,11 @@
       <c r="CT73" s="2">
         <v>97266</v>
       </c>
+      <c r="CU73" s="2">
+        <v>98222</v>
+      </c>
     </row>
-    <row r="74" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -23484,8 +23700,11 @@
       <c r="CT74" s="2">
         <v>14521</v>
       </c>
+      <c r="CU74" s="2">
+        <v>14685</v>
+      </c>
     </row>
-    <row r="75" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -23780,8 +23999,11 @@
       <c r="CT75" s="2">
         <v>9527</v>
       </c>
+      <c r="CU75" s="2">
+        <v>9622</v>
+      </c>
     </row>
-    <row r="76" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -24076,8 +24298,11 @@
       <c r="CT76" s="2">
         <v>16783</v>
       </c>
+      <c r="CU76" s="2">
+        <v>16917</v>
+      </c>
     </row>
-    <row r="77" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -24372,8 +24597,11 @@
       <c r="CT77" s="2">
         <v>10035</v>
       </c>
+      <c r="CU77" s="2">
+        <v>10135</v>
+      </c>
     </row>
-    <row r="78" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -24668,8 +24896,11 @@
       <c r="CT78" s="2">
         <v>1071</v>
       </c>
+      <c r="CU78" s="2">
+        <v>1086</v>
+      </c>
     </row>
-    <row r="79" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -24964,8 +25195,11 @@
       <c r="CT79" s="2">
         <v>1882</v>
       </c>
+      <c r="CU79" s="2">
+        <v>1896</v>
+      </c>
     </row>
-    <row r="80" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -25260,8 +25494,11 @@
       <c r="CT80" s="2">
         <v>638</v>
       </c>
+      <c r="CU80" s="2">
+        <v>640</v>
+      </c>
     </row>
-    <row r="81" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -25556,8 +25793,11 @@
       <c r="CT81" s="2">
         <v>380167</v>
       </c>
+      <c r="CU81" s="2">
+        <v>382943</v>
+      </c>
     </row>
-    <row r="82" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -25852,8 +26092,11 @@
       <c r="CT82" s="2">
         <v>3102</v>
       </c>
+      <c r="CU82" s="2">
+        <v>3143</v>
+      </c>
     </row>
-    <row r="83" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -26148,8 +26391,11 @@
       <c r="CT83" s="2">
         <v>11025</v>
       </c>
+      <c r="CU83" s="2">
+        <v>11157</v>
+      </c>
     </row>
-    <row r="84" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -26444,8 +26690,11 @@
       <c r="CT84" s="2">
         <v>10216</v>
       </c>
+      <c r="CU84" s="2">
+        <v>10256</v>
+      </c>
     </row>
-    <row r="85" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -26740,8 +26989,11 @@
       <c r="CT85" s="2">
         <v>3208</v>
       </c>
+      <c r="CU85" s="2">
+        <v>3236</v>
+      </c>
     </row>
-    <row r="86" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -27036,8 +27288,11 @@
       <c r="CT86" s="2">
         <v>222046</v>
       </c>
+      <c r="CU86" s="2">
+        <v>224399</v>
+      </c>
     </row>
-    <row r="87" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -27332,8 +27587,11 @@
       <c r="CT87" s="2">
         <v>2020</v>
       </c>
+      <c r="CU87" s="2">
+        <v>2026</v>
+      </c>
     </row>
-    <row r="88" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -27628,8 +27886,11 @@
       <c r="CT88" s="2">
         <v>12148</v>
       </c>
+      <c r="CU88" s="2">
+        <v>12229</v>
+      </c>
     </row>
-    <row r="89" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>86</v>
       </c>
@@ -27924,8 +28185,11 @@
       <c r="CT89" s="2">
         <v>136</v>
       </c>
+      <c r="CU89" s="2">
+        <v>137</v>
+      </c>
     </row>
-    <row r="90" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -28220,8 +28484,11 @@
       <c r="CT90" s="2">
         <v>2469</v>
       </c>
+      <c r="CU90" s="2">
+        <v>2477</v>
+      </c>
     </row>
-    <row r="91" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>88</v>
       </c>
@@ -28516,8 +28783,11 @@
       <c r="CT91" s="2">
         <v>9457</v>
       </c>
+      <c r="CU91" s="2">
+        <v>9589</v>
+      </c>
     </row>
-    <row r="92" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -28812,8 +29082,11 @@
       <c r="CT92" s="2">
         <v>6490</v>
       </c>
+      <c r="CU92" s="2">
+        <v>6502</v>
+      </c>
     </row>
-    <row r="93" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -29108,8 +29381,11 @@
       <c r="CT93" s="2">
         <v>64015</v>
       </c>
+      <c r="CU93" s="2">
+        <v>64415</v>
+      </c>
     </row>
-    <row r="94" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>91</v>
       </c>
@@ -29404,8 +29680,11 @@
       <c r="CT94" s="2">
         <v>41417</v>
       </c>
+      <c r="CU94" s="2">
+        <v>41944</v>
+      </c>
     </row>
-    <row r="95" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -29700,8 +29979,11 @@
       <c r="CT95" s="2">
         <v>15498</v>
       </c>
+      <c r="CU95" s="2">
+        <v>15958</v>
+      </c>
     </row>
-    <row r="96" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -29996,8 +30278,11 @@
       <c r="CT96" s="2">
         <v>46130</v>
       </c>
+      <c r="CU96" s="2">
+        <v>46650</v>
+      </c>
     </row>
-    <row r="97" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>94</v>
       </c>
@@ -30292,8 +30577,11 @@
       <c r="CT97" s="2">
         <v>10459</v>
       </c>
+      <c r="CU97" s="2">
+        <v>10529</v>
+      </c>
     </row>
-    <row r="98" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -30588,8 +30876,11 @@
       <c r="CT98" s="2">
         <v>1868</v>
       </c>
+      <c r="CU98" s="2">
+        <v>1873</v>
+      </c>
     </row>
-    <row r="99" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -30884,8 +31175,11 @@
       <c r="CT99" s="2">
         <v>3692</v>
       </c>
+      <c r="CU99" s="2">
+        <v>3742</v>
+      </c>
     </row>
-    <row r="100" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -31180,8 +31474,11 @@
       <c r="CT100" s="2">
         <v>2000</v>
       </c>
+      <c r="CU100" s="2">
+        <v>2000</v>
+      </c>
     </row>
-    <row r="101" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -31476,8 +31773,11 @@
       <c r="CT101" s="2">
         <v>1513</v>
       </c>
+      <c r="CU101" s="2">
+        <v>1514</v>
+      </c>
     </row>
-    <row r="102" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -31772,8 +32072,11 @@
       <c r="CT102" s="2">
         <v>15991</v>
       </c>
+      <c r="CU102" s="2">
+        <v>16217</v>
+      </c>
     </row>
-    <row r="103" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>100</v>
       </c>
@@ -32068,8 +32371,11 @@
       <c r="CT103" s="2">
         <v>2383859</v>
       </c>
+      <c r="CU103" s="2">
+        <v>2399205</v>
+      </c>
     </row>
-    <row r="104" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -32364,8 +32670,11 @@
       <c r="CT104" s="2">
         <v>42992</v>
       </c>
+      <c r="CU104" s="2">
+        <v>43528</v>
+      </c>
     </row>
-    <row r="105" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -32660,8 +32969,11 @@
       <c r="CT105" s="2">
         <v>133</v>
       </c>
+      <c r="CU105" s="2">
+        <v>133</v>
+      </c>
     </row>
-    <row r="106" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>103</v>
       </c>
@@ -32956,8 +33268,11 @@
       <c r="CT106" s="2">
         <v>1717</v>
       </c>
+      <c r="CU106" s="2">
+        <v>1719</v>
+      </c>
     </row>
-    <row r="107" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>104</v>
       </c>
@@ -33252,8 +33567,11 @@
       <c r="CT107" s="2">
         <v>129427</v>
       </c>
+      <c r="CU107" s="2">
+        <v>131324</v>
+      </c>
     </row>
-    <row r="108" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>105</v>
       </c>
@@ -33548,8 +33866,11 @@
       <c r="CT108" s="2">
         <v>979</v>
       </c>
+      <c r="CU108" s="2">
+        <v>981</v>
+      </c>
     </row>
-    <row r="109" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>106</v>
       </c>
@@ -33844,8 +34165,11 @@
       <c r="CT109" s="2">
         <v>19614</v>
       </c>
+      <c r="CU109" s="2">
+        <v>19791</v>
+      </c>
     </row>
-    <row r="110" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -34140,8 +34464,11 @@
       <c r="CT110" s="2">
         <v>317935</v>
       </c>
+      <c r="CU110" s="2">
+        <v>319990</v>
+      </c>
     </row>
-    <row r="111" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>108</v>
       </c>
@@ -34436,8 +34763,11 @@
       <c r="CT111" s="2">
         <v>25225</v>
       </c>
+      <c r="CU111" s="2">
+        <v>25563</v>
+      </c>
     </row>
-    <row r="112" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>109</v>
       </c>
@@ -34732,8 +35062,11 @@
       <c r="CT112" s="2">
         <v>7320</v>
       </c>
+      <c r="CU112" s="2">
+        <v>7377</v>
+      </c>
     </row>
-    <row r="113" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -35028,8 +35361,11 @@
       <c r="CT113" s="2">
         <v>30765</v>
       </c>
+      <c r="CU113" s="2">
+        <v>31146</v>
+      </c>
     </row>
-    <row r="114" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>111</v>
       </c>
@@ -35324,8 +35660,11 @@
       <c r="CT114" s="2">
         <v>12557</v>
       </c>
+      <c r="CU114" s="2">
+        <v>12698</v>
+      </c>
     </row>
-    <row r="115" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>112</v>
       </c>
@@ -35620,8 +35959,11 @@
       <c r="CT115" s="2">
         <v>11672</v>
       </c>
+      <c r="CU115" s="2">
+        <v>11724</v>
+      </c>
     </row>
-    <row r="116" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -35916,8 +36258,11 @@
       <c r="CT116" s="2">
         <v>11317</v>
       </c>
+      <c r="CU116" s="2">
+        <v>11485</v>
+      </c>
     </row>
-    <row r="117" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -36212,8 +36557,11 @@
       <c r="CT117" s="2">
         <v>1956</v>
       </c>
+      <c r="CU117" s="2">
+        <v>2028</v>
+      </c>
     </row>
-    <row r="118" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>115</v>
       </c>
@@ -36508,8 +36856,11 @@
       <c r="CT118" s="2">
         <v>46495</v>
       </c>
+      <c r="CU118" s="2">
+        <v>46913</v>
+      </c>
     </row>
-    <row r="119" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -36804,8 +37155,11 @@
       <c r="CT119" s="2">
         <v>8253</v>
       </c>
+      <c r="CU119" s="2">
+        <v>8353</v>
+      </c>
     </row>
-    <row r="120" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>117</v>
       </c>
@@ -37100,8 +37454,11 @@
       <c r="CT120" s="2">
         <v>370</v>
       </c>
+      <c r="CU120" s="2">
+        <v>371</v>
+      </c>
     </row>
-    <row r="121" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -37396,8 +37753,11 @@
       <c r="CT121" s="2">
         <v>1151</v>
       </c>
+      <c r="CU121" s="2">
+        <v>1156</v>
+      </c>
     </row>
-    <row r="122" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>119</v>
       </c>
@@ -37692,8 +38052,11 @@
       <c r="CT122" s="2">
         <v>5350</v>
       </c>
+      <c r="CU122" s="2">
+        <v>5370</v>
+      </c>
     </row>
-    <row r="123" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -37988,8 +38351,11 @@
       <c r="CT123" s="2">
         <v>10768</v>
       </c>
+      <c r="CU123" s="2">
+        <v>10886</v>
+      </c>
     </row>
-    <row r="124" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -38284,8 +38650,11 @@
       <c r="CT124" s="2">
         <v>1310</v>
       </c>
+      <c r="CU124" s="2">
+        <v>1319</v>
+      </c>
     </row>
-    <row r="125" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -38580,8 +38949,11 @@
       <c r="CT125" s="2">
         <v>129084</v>
       </c>
+      <c r="CU125" s="2">
+        <v>129760</v>
+      </c>
     </row>
-    <row r="126" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -38876,8 +39248,11 @@
       <c r="CT126" s="2">
         <v>7171</v>
       </c>
+      <c r="CU126" s="2">
+        <v>7192</v>
+      </c>
     </row>
-    <row r="127" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>124</v>
       </c>
@@ -39172,8 +39547,11 @@
       <c r="CT127" s="2">
         <v>39242</v>
       </c>
+      <c r="CU127" s="2">
+        <v>39627</v>
+      </c>
     </row>
-    <row r="128" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>125</v>
       </c>
@@ -39468,8 +39846,11 @@
       <c r="CT128" s="2">
         <v>75261</v>
       </c>
+      <c r="CU128" s="2">
+        <v>75749</v>
+      </c>
     </row>
-    <row r="129" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>126</v>
       </c>
@@ -39764,8 +40145,11 @@
       <c r="CT129" s="2">
         <v>5237</v>
       </c>
+      <c r="CU129" s="2">
+        <v>5277</v>
+      </c>
     </row>
-    <row r="130" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>127</v>
       </c>
@@ -40060,8 +40444,11 @@
       <c r="CT130" s="2">
         <v>10731</v>
       </c>
+      <c r="CU130" s="2">
+        <v>10852</v>
+      </c>
     </row>
-    <row r="131" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>128</v>
       </c>
@@ -40356,8 +40743,11 @@
       <c r="CT131" s="2">
         <v>65351</v>
       </c>
+      <c r="CU131" s="2">
+        <v>66072</v>
+      </c>
     </row>
-    <row r="132" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>129</v>
       </c>
@@ -40652,8 +41042,11 @@
       <c r="CT132" s="2">
         <v>15238</v>
       </c>
+      <c r="CU132" s="2">
+        <v>15370</v>
+      </c>
     </row>
-    <row r="133" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>130</v>
       </c>
@@ -40948,8 +41341,11 @@
       <c r="CT133" s="2">
         <v>148</v>
       </c>
+      <c r="CU133" s="2">
+        <v>148</v>
+      </c>
     </row>
-    <row r="134" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>131</v>
       </c>
@@ -41244,8 +41640,11 @@
       <c r="CT134" s="2">
         <v>388</v>
       </c>
+      <c r="CU134" s="2">
+        <v>389</v>
+      </c>
     </row>
-    <row r="135" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>132</v>
       </c>
@@ -41540,8 +41939,11 @@
       <c r="CT135" s="2">
         <v>29541</v>
       </c>
+      <c r="CU135" s="2">
+        <v>30027</v>
+      </c>
     </row>
-    <row r="136" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>133</v>
       </c>
@@ -41836,8 +42238,11 @@
       <c r="CT136" s="2">
         <v>1468</v>
       </c>
+      <c r="CU136" s="2">
+        <v>1476</v>
+      </c>
     </row>
-    <row r="137" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -42132,8 +42537,11 @@
       <c r="CT137" s="2">
         <v>37</v>
       </c>
+      <c r="CU137" s="2">
+        <v>37</v>
+      </c>
     </row>
-    <row r="138" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>135</v>
       </c>
@@ -42428,8 +42836,11 @@
       <c r="CT138" s="2">
         <v>1049</v>
       </c>
+      <c r="CU138" s="2">
+        <v>1144</v>
+      </c>
     </row>
-    <row r="139" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>136</v>
       </c>
@@ -42724,8 +43135,11 @@
       <c r="CT139" s="2">
         <v>22242</v>
       </c>
+      <c r="CU139" s="2">
+        <v>22370</v>
+      </c>
     </row>
-    <row r="140" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>137</v>
       </c>
@@ -43020,8 +43434,11 @@
       <c r="CT140" s="2">
         <v>1537</v>
       </c>
+      <c r="CU140" s="2">
+        <v>1539</v>
+      </c>
     </row>
-    <row r="141" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>138</v>
       </c>
@@ -43316,8 +43733,11 @@
       <c r="CT141" s="2">
         <v>4800</v>
       </c>
+      <c r="CU141" s="2">
+        <v>4830</v>
+      </c>
     </row>
-    <row r="142" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>139</v>
       </c>
@@ -43612,8 +44032,11 @@
       <c r="CT142" s="2">
         <v>15519</v>
       </c>
+      <c r="CU142" s="2">
+        <v>15626</v>
+      </c>
     </row>
-    <row r="143" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>140</v>
       </c>
@@ -43908,8 +44331,11 @@
       <c r="CT143" s="2">
         <v>6518</v>
       </c>
+      <c r="CU143" s="2">
+        <v>6557</v>
+      </c>
     </row>
-    <row r="144" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>141</v>
       </c>
@@ -44204,8 +44630,11 @@
       <c r="CT144" s="2">
         <v>11411</v>
       </c>
+      <c r="CU144" s="2">
+        <v>11510</v>
+      </c>
     </row>
-    <row r="145" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>142</v>
       </c>
@@ -44500,8 +44929,11 @@
       <c r="CT145" s="2">
         <v>9186</v>
       </c>
+      <c r="CU145" s="2">
+        <v>9211</v>
+      </c>
     </row>
-    <row r="146" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>143</v>
       </c>
@@ -44796,8 +45228,11 @@
       <c r="CT146" s="2">
         <v>5525</v>
       </c>
+      <c r="CU146" s="2">
+        <v>5759</v>
+      </c>
     </row>
-    <row r="147" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>144</v>
       </c>
@@ -45092,8 +45527,11 @@
       <c r="CT147" s="2">
         <v>6444</v>
       </c>
+      <c r="CU147" s="2">
+        <v>6537</v>
+      </c>
     </row>
-    <row r="148" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>145</v>
       </c>
@@ -45388,8 +45826,11 @@
       <c r="CT148" s="2">
         <v>34631</v>
       </c>
+      <c r="CU148" s="2">
+        <v>34917</v>
+      </c>
     </row>
-    <row r="149" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>146</v>
       </c>
@@ -45684,8 +46125,11 @@
       <c r="CT149" s="2">
         <v>17982</v>
       </c>
+      <c r="CU149" s="2">
+        <v>18325</v>
+      </c>
     </row>
-    <row r="150" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>147</v>
       </c>
@@ -45980,8 +46424,11 @@
       <c r="CT150" s="2">
         <v>256</v>
       </c>
+      <c r="CU150" s="2">
+        <v>257</v>
+      </c>
     </row>
-    <row r="151" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>148</v>
       </c>
@@ -46276,8 +46723,11 @@
       <c r="CT151" s="2">
         <v>3417</v>
       </c>
+      <c r="CU151" s="2">
+        <v>3473</v>
+      </c>
     </row>
-    <row r="152" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>149</v>
       </c>
@@ -46572,8 +47022,11 @@
       <c r="CT152" s="2">
         <v>6983</v>
       </c>
+      <c r="CU152" s="2">
+        <v>7052</v>
+      </c>
     </row>
-    <row r="153" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>150</v>
       </c>
@@ -46868,8 +47321,11 @@
       <c r="CT153" s="2">
         <v>23</v>
       </c>
+      <c r="CU153" s="2">
+        <v>23</v>
+      </c>
     </row>
-    <row r="154" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>151</v>
       </c>
@@ -47164,8 +47620,11 @@
       <c r="CT154" s="2">
         <v>203220</v>
       </c>
+      <c r="CU154" s="2">
+        <v>204727</v>
+      </c>
     </row>
-    <row r="155" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -47460,8 +47919,11 @@
       <c r="CT155" s="2">
         <v>2968</v>
       </c>
+      <c r="CU155" s="2">
+        <v>2988</v>
+      </c>
     </row>
-    <row r="156" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>153</v>
       </c>
@@ -47756,8 +48218,11 @@
       <c r="CT156" s="2">
         <v>9681</v>
       </c>
+      <c r="CU156" s="2">
+        <v>9764</v>
+      </c>
     </row>
-    <row r="157" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>154</v>
       </c>
@@ -48052,8 +48517,11 @@
       <c r="CT157" s="2">
         <v>2225</v>
       </c>
+      <c r="CU157" s="2">
+        <v>2250</v>
+      </c>
     </row>
-    <row r="158" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>155</v>
       </c>
@@ -48348,8 +48816,11 @@
       <c r="CT158" s="2">
         <v>1230</v>
       </c>
+      <c r="CU158" s="2">
+        <v>1248</v>
+      </c>
     </row>
-    <row r="159" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -48644,8 +49115,11 @@
       <c r="CT159" s="2">
         <v>1517</v>
       </c>
+      <c r="CU159" s="2">
+        <v>1541</v>
+      </c>
     </row>
-    <row r="160" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>157</v>
       </c>
@@ -48940,8 +49414,11 @@
       <c r="CT160" s="2">
         <v>15881</v>
       </c>
+      <c r="CU160" s="2">
+        <v>16084</v>
+      </c>
     </row>
-    <row r="161" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>158</v>
       </c>
@@ -49236,8 +49713,11 @@
       <c r="CT161" s="2">
         <v>34838</v>
       </c>
+      <c r="CU161" s="2">
+        <v>35326</v>
+      </c>
     </row>
-    <row r="162" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>159</v>
       </c>
@@ -49532,8 +50012,11 @@
       <c r="CT162" s="2">
         <v>2231</v>
       </c>
+      <c r="CU162" s="2">
+        <v>2253</v>
+      </c>
     </row>
-    <row r="163" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>160</v>
       </c>
@@ -49828,8 +50311,11 @@
       <c r="CT163" s="2">
         <v>183149</v>
       </c>
+      <c r="CU163" s="2">
+        <v>184674</v>
+      </c>
     </row>
-    <row r="164" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>161</v>
       </c>
@@ -50124,8 +50610,11 @@
       <c r="CT164" s="2">
         <v>268</v>
       </c>
+      <c r="CU164" s="2">
+        <v>273</v>
+      </c>
     </row>
-    <row r="165" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>162</v>
       </c>
@@ -50420,8 +50909,11 @@
       <c r="CT165" s="2">
         <v>17278</v>
       </c>
+      <c r="CU165" s="2">
+        <v>17407</v>
+      </c>
     </row>
-    <row r="166" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>163</v>
       </c>
@@ -50716,8 +51208,11 @@
       <c r="CT166" s="2">
         <v>1763</v>
       </c>
+      <c r="CU166" s="2">
+        <v>1773</v>
+      </c>
     </row>
-    <row r="167" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>164</v>
       </c>
@@ -51012,8 +51507,11 @@
       <c r="CT167" s="2">
         <v>50380</v>
       </c>
+      <c r="CU167" s="2">
+        <v>51167</v>
+      </c>
     </row>
-    <row r="168" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>165</v>
       </c>
@@ -51308,8 +51806,11 @@
       <c r="CT168" s="2">
         <v>11983</v>
       </c>
+      <c r="CU168" s="2">
+        <v>12080</v>
+      </c>
     </row>
-    <row r="169" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>166</v>
       </c>
@@ -51604,8 +52105,11 @@
       <c r="CT169" s="2">
         <v>3374</v>
       </c>
+      <c r="CU169" s="2">
+        <v>3382</v>
+      </c>
     </row>
-    <row r="170" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>167</v>
       </c>
@@ -51900,8 +52404,11 @@
       <c r="CT170" s="2">
         <v>4713</v>
       </c>
+      <c r="CU170" s="2">
+        <v>4740</v>
+      </c>
     </row>
-    <row r="171" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>168</v>
       </c>
@@ -52196,8 +52703,11 @@
       <c r="CT171" s="2">
         <v>7859</v>
       </c>
+      <c r="CU171" s="2">
+        <v>7932</v>
+      </c>
     </row>
-    <row r="172" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>169</v>
       </c>
@@ -52492,8 +53002,11 @@
       <c r="CT172" s="2">
         <v>220903</v>
       </c>
+      <c r="CU172" s="2">
+        <v>222565</v>
+      </c>
     </row>
-    <row r="173" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>170</v>
       </c>
@@ -52788,8 +53301,11 @@
       <c r="CT173" s="2">
         <v>6911</v>
       </c>
+      <c r="CU173" s="2">
+        <v>6916</v>
+      </c>
     </row>
-    <row r="174" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>171</v>
       </c>
@@ -53084,8 +53600,11 @@
       <c r="CT174" s="2">
         <v>4911</v>
       </c>
+      <c r="CU174" s="2">
+        <v>4965</v>
+      </c>
     </row>
-    <row r="175" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>172</v>
       </c>
@@ -53380,8 +53899,11 @@
       <c r="CT175" s="2">
         <v>458</v>
       </c>
+      <c r="CU175" s="2">
+        <v>459</v>
+      </c>
     </row>
-    <row r="176" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>173</v>
       </c>
@@ -53676,8 +54198,11 @@
       <c r="CT176" s="2">
         <v>29356</v>
       </c>
+      <c r="CU176" s="2">
+        <v>29722</v>
+      </c>
     </row>
-    <row r="177" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>174</v>
       </c>
@@ -53972,8 +54497,11 @@
       <c r="CT177" s="2">
         <v>21077</v>
       </c>
+      <c r="CU177" s="2">
+        <v>21241</v>
+      </c>
     </row>
-    <row r="178" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>175</v>
       </c>
@@ -54268,8 +54796,11 @@
       <c r="CT178" s="2">
         <v>3258</v>
       </c>
+      <c r="CU178" s="2">
+        <v>3287</v>
+      </c>
     </row>
-    <row r="179" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>176</v>
       </c>
@@ -54564,8 +55095,11 @@
       <c r="CT179" s="2">
         <v>6186</v>
       </c>
+      <c r="CU179" s="2">
+        <v>6290</v>
+      </c>
     </row>
-    <row r="180" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>177</v>
       </c>
@@ -54860,8 +55394,11 @@
       <c r="CT180" s="2">
         <v>182292</v>
       </c>
+      <c r="CU180" s="2">
+        <v>184054</v>
+      </c>
     </row>
-    <row r="181" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>178</v>
       </c>
@@ -55156,8 +55693,11 @@
       <c r="CT181" s="2">
         <v>513</v>
       </c>
+      <c r="CU181" s="2">
+        <v>514</v>
+      </c>
     </row>
-    <row r="182" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>179</v>
       </c>
@@ -55452,8 +55992,11 @@
       <c r="CT182" s="2">
         <v>652</v>
       </c>
+      <c r="CU182" s="2">
+        <v>655</v>
+      </c>
     </row>
-    <row r="183" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>180</v>
       </c>
@@ -55748,8 +56291,11 @@
       <c r="CT183" s="2">
         <v>23077</v>
       </c>
+      <c r="CU183" s="2">
+        <v>23392</v>
+      </c>
     </row>
-    <row r="184" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>181</v>
       </c>
@@ -56044,8 +56590,11 @@
       <c r="CT184" s="2">
         <v>9827</v>
       </c>
+      <c r="CU184" s="2">
+        <v>9904</v>
+      </c>
     </row>
-    <row r="185" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>182</v>
       </c>
@@ -56340,8 +56889,11 @@
       <c r="CT185" s="2">
         <v>6585</v>
       </c>
+      <c r="CU185" s="2">
+        <v>6641</v>
+      </c>
     </row>
-    <row r="186" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>183</v>
       </c>
@@ -56636,8 +57188,11 @@
       <c r="CT186" s="2">
         <v>45629</v>
       </c>
+      <c r="CU186" s="2">
+        <v>46004</v>
+      </c>
     </row>
-    <row r="187" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>184</v>
       </c>
@@ -56932,8 +57487,11 @@
       <c r="CT187" s="2">
         <v>1949</v>
       </c>
+      <c r="CU187" s="2">
+        <v>1955</v>
+      </c>
     </row>
-    <row r="188" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>185</v>
       </c>
@@ -57228,8 +57786,11 @@
       <c r="CT188" s="2">
         <v>7012</v>
       </c>
+      <c r="CU188" s="2">
+        <v>7087</v>
+      </c>
     </row>
-    <row r="189" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>186</v>
       </c>
@@ -57524,8 +58085,11 @@
       <c r="CT189" s="2">
         <v>21024</v>
       </c>
+      <c r="CU189" s="2">
+        <v>21144</v>
+      </c>
     </row>
-    <row r="190" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>187</v>
       </c>
@@ -57820,8 +58384,11 @@
       <c r="CT190" s="2">
         <v>58574</v>
       </c>
+      <c r="CU190" s="2">
+        <v>58697</v>
+      </c>
     </row>
-    <row r="191" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>188</v>
       </c>
@@ -58116,8 +58683,11 @@
       <c r="CT191" s="2">
         <v>6158</v>
       </c>
+      <c r="CU191" s="2">
+        <v>6175</v>
+      </c>
     </row>
-    <row r="192" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>189</v>
       </c>
@@ -58412,8 +58982,11 @@
       <c r="CT192" s="2">
         <v>2018</v>
       </c>
+      <c r="CU192" s="2">
+        <v>2046</v>
+      </c>
     </row>
-    <row r="193" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>190</v>
       </c>
@@ -58708,8 +59281,11 @@
       <c r="CT193" s="2">
         <v>40084</v>
       </c>
+      <c r="CU193" s="2">
+        <v>40260</v>
+      </c>
     </row>
-    <row r="194" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>191</v>
       </c>
@@ -59004,8 +59580,11 @@
       <c r="CT194" s="2">
         <v>1001</v>
       </c>
+      <c r="CU194" s="2">
+        <v>1003</v>
+      </c>
     </row>
-    <row r="195" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>192</v>
       </c>
@@ -59300,8 +59879,11 @@
       <c r="CT195" s="2">
         <v>1242</v>
       </c>
+      <c r="CU195" s="2">
+        <v>1275</v>
+      </c>
     </row>
-    <row r="196" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>193</v>
       </c>
@@ -59596,8 +60178,11 @@
       <c r="CT196" s="2">
         <v>4358</v>
       </c>
+      <c r="CU196" s="2">
+        <v>4400</v>
+      </c>
     </row>
-    <row r="197" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>194</v>
       </c>
@@ -59892,8 +60477,11 @@
       <c r="CT197" s="2">
         <v>3632</v>
       </c>
+      <c r="CU197" s="2">
+        <v>3637</v>
+      </c>
     </row>
-    <row r="198" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>195</v>
       </c>
@@ -60188,8 +60776,11 @@
       <c r="CT198" s="2">
         <v>3953</v>
       </c>
+      <c r="CU198" s="2">
+        <v>3972</v>
+      </c>
     </row>
-    <row r="199" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>196</v>
       </c>
@@ -60484,8 +61075,11 @@
       <c r="CT199" s="2">
         <v>114</v>
       </c>
+      <c r="CU199" s="2">
+        <v>114</v>
+      </c>
     </row>
-    <row r="200" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>197</v>
       </c>
@@ -60780,8 +61374,11 @@
       <c r="CT200" s="2">
         <v>9134</v>
       </c>
+      <c r="CU200" s="2">
+        <v>9245</v>
+      </c>
     </row>
-    <row r="201" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>198</v>
       </c>
@@ -61076,8 +61673,11 @@
       <c r="CT201" s="2">
         <v>42716</v>
       </c>
+      <c r="CU201" s="2">
+        <v>42936</v>
+      </c>
     </row>
-    <row r="202" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>199</v>
       </c>
@@ -61372,8 +61972,11 @@
       <c r="CT202" s="2">
         <v>5243</v>
       </c>
+      <c r="CU202" s="2">
+        <v>5267</v>
+      </c>
     </row>
-    <row r="203" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>200</v>
       </c>
@@ -61668,8 +62271,11 @@
       <c r="CT203" s="2">
         <v>14093</v>
       </c>
+      <c r="CU203" s="2">
+        <v>14227</v>
+      </c>
     </row>
-    <row r="204" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>201</v>
       </c>
@@ -61964,8 +62570,11 @@
       <c r="CT204" s="2">
         <v>4493</v>
       </c>
+      <c r="CU204" s="2">
+        <v>4530</v>
+      </c>
     </row>
-    <row r="205" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>202</v>
       </c>
@@ -62260,8 +62869,11 @@
       <c r="CT205" s="2">
         <v>4313</v>
       </c>
+      <c r="CU205" s="2">
+        <v>4447</v>
+      </c>
     </row>
-    <row r="206" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>203</v>
       </c>
@@ -62556,8 +63168,11 @@
       <c r="CT206" s="2">
         <v>10788</v>
       </c>
+      <c r="CU206" s="2">
+        <v>10868</v>
+      </c>
     </row>
-    <row r="207" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>204</v>
       </c>
@@ -62852,8 +63467,11 @@
       <c r="CT207" s="2">
         <v>28237</v>
       </c>
+      <c r="CU207" s="2">
+        <v>28482</v>
+      </c>
     </row>
-    <row r="208" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>205</v>
       </c>
@@ -63148,8 +63766,11 @@
       <c r="CT208" s="2">
         <v>2434</v>
       </c>
+      <c r="CU208" s="2">
+        <v>2443</v>
+      </c>
     </row>
-    <row r="209" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>206</v>
       </c>
@@ -63444,8 +64065,11 @@
       <c r="CT209" s="2">
         <v>901</v>
       </c>
+      <c r="CU209" s="2">
+        <v>906</v>
+      </c>
     </row>
-    <row r="210" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>207</v>
       </c>
@@ -63740,8 +64364,11 @@
       <c r="CT210" s="2">
         <v>13201</v>
       </c>
+      <c r="CU210" s="2">
+        <v>13315</v>
+      </c>
     </row>
-    <row r="211" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>208</v>
       </c>
@@ -64036,8 +64663,11 @@
       <c r="CT211" s="2">
         <v>727</v>
       </c>
+      <c r="CU211" s="2">
+        <v>729</v>
+      </c>
     </row>
-    <row r="212" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>209</v>
       </c>
@@ -64332,8 +64962,11 @@
       <c r="CT212" s="2">
         <v>9334</v>
       </c>
+      <c r="CU212" s="2">
+        <v>9397</v>
+      </c>
     </row>
-    <row r="213" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>210</v>
       </c>
@@ -64628,8 +65261,11 @@
       <c r="CT213" s="2">
         <v>158</v>
       </c>
+      <c r="CU213" s="2">
+        <v>158</v>
+      </c>
     </row>
-    <row r="214" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>211</v>
       </c>
@@ -64924,8 +65560,11 @@
       <c r="CT214" s="2">
         <v>123538</v>
       </c>
+      <c r="CU214" s="2">
+        <v>125147</v>
+      </c>
     </row>
-    <row r="215" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>212</v>
       </c>
@@ -65220,8 +65859,11 @@
       <c r="CT215" s="2">
         <v>4960</v>
       </c>
+      <c r="CU215" s="2">
+        <v>5016</v>
+      </c>
     </row>
-    <row r="216" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>213</v>
       </c>
@@ -65516,8 +66158,11 @@
       <c r="CT216" s="2">
         <v>26413</v>
       </c>
+      <c r="CU216" s="2">
+        <v>26927</v>
+      </c>
     </row>
-    <row r="217" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>214</v>
       </c>
@@ -65812,8 +66457,11 @@
       <c r="CT217" s="2">
         <v>2335</v>
       </c>
+      <c r="CU217" s="2">
+        <v>2351</v>
+      </c>
     </row>
-    <row r="218" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>215</v>
       </c>
@@ -66108,8 +66756,11 @@
       <c r="CT218" s="2">
         <v>678</v>
       </c>
+      <c r="CU218" s="2">
+        <v>680</v>
+      </c>
     </row>
-    <row r="219" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>216</v>
       </c>
@@ -66404,8 +67055,11 @@
       <c r="CT219" s="2">
         <v>213</v>
       </c>
+      <c r="CU219" s="2">
+        <v>215</v>
+      </c>
     </row>
-    <row r="220" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>217</v>
       </c>
@@ -66700,8 +67354,11 @@
       <c r="CT220" s="2">
         <v>1328</v>
       </c>
+      <c r="CU220" s="2">
+        <v>1344</v>
+      </c>
     </row>
-    <row r="221" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>218</v>
       </c>
@@ -66996,8 +67653,11 @@
       <c r="CT221" s="2">
         <v>3184</v>
       </c>
+      <c r="CU221" s="2">
+        <v>3203</v>
+      </c>
     </row>
-    <row r="222" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>219</v>
       </c>
@@ -67292,8 +67952,11 @@
       <c r="CT222" s="2">
         <v>971449</v>
       </c>
+      <c r="CU222" s="2">
+        <v>979250</v>
+      </c>
     </row>
-    <row r="223" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>220</v>
       </c>
@@ -67588,8 +68251,11 @@
       <c r="CT223" s="2">
         <v>74461</v>
       </c>
+      <c r="CU223" s="2">
+        <v>75333</v>
+      </c>
     </row>
-    <row r="224" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>221</v>
       </c>
@@ -67884,8 +68550,11 @@
       <c r="CT224" s="2">
         <v>283</v>
       </c>
+      <c r="CU224" s="2">
+        <v>287</v>
+      </c>
     </row>
-    <row r="225" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>222</v>
       </c>
@@ -68180,8 +68849,11 @@
       <c r="CT225" s="2">
         <v>3088</v>
       </c>
+      <c r="CU225" s="2">
+        <v>3097</v>
+      </c>
     </row>
-    <row r="226" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>223</v>
       </c>
@@ -68476,8 +69148,11 @@
       <c r="CT226" s="2">
         <v>219</v>
       </c>
+      <c r="CU226" s="2">
+        <v>219</v>
+      </c>
     </row>
-    <row r="227" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>224</v>
       </c>
@@ -68772,8 +69447,11 @@
       <c r="CT227" s="2">
         <v>15181</v>
       </c>
+      <c r="CU227" s="2">
+        <v>15433</v>
+      </c>
     </row>
-    <row r="228" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>225</v>
       </c>
@@ -69068,8 +69746,11 @@
       <c r="CT228" s="2">
         <v>72959</v>
       </c>
+      <c r="CU228" s="2">
+        <v>73446</v>
+      </c>
     </row>
-    <row r="229" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>226</v>
       </c>
@@ -69364,8 +70045,11 @@
       <c r="CT229" s="2">
         <v>595771</v>
       </c>
+      <c r="CU229" s="2">
+        <v>603608</v>
+      </c>
     </row>
-    <row r="230" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>227</v>
       </c>
@@ -69660,8 +70344,11 @@
       <c r="CT230" s="2">
         <v>6435</v>
       </c>
+      <c r="CU230" s="2">
+        <v>6565</v>
+      </c>
     </row>
-    <row r="231" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>228</v>
       </c>
@@ -69956,8 +70643,11 @@
       <c r="CT231" s="2">
         <v>8497</v>
       </c>
+      <c r="CU231" s="2">
+        <v>8613</v>
+      </c>
     </row>
-    <row r="232" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>229</v>
       </c>
@@ -70252,8 +70942,11 @@
       <c r="CT232" s="2">
         <v>8744</v>
       </c>
+      <c r="CU232" s="2">
+        <v>8829</v>
+      </c>
     </row>
-    <row r="233" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>230</v>
       </c>
@@ -70548,8 +71241,11 @@
       <c r="CT233" s="2">
         <v>1487</v>
       </c>
+      <c r="CU233" s="2">
+        <v>1508</v>
+      </c>
     </row>
-    <row r="234" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>231</v>
       </c>
@@ -70844,8 +71540,11 @@
       <c r="CT234" s="2">
         <v>12902</v>
       </c>
+      <c r="CU234" s="2">
+        <v>13247</v>
+      </c>
     </row>
-    <row r="235" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>232</v>
       </c>
@@ -71140,8 +71839,11 @@
       <c r="CT235" s="2">
         <v>25477</v>
       </c>
+      <c r="CU235" s="2">
+        <v>25865</v>
+      </c>
     </row>
-    <row r="236" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>233</v>
       </c>
@@ -71436,8 +72138,11 @@
       <c r="CT236" s="2">
         <v>13162</v>
       </c>
+      <c r="CU236" s="2">
+        <v>13276</v>
+      </c>
     </row>
-    <row r="237" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>234</v>
       </c>
@@ -71732,8 +72437,11 @@
       <c r="CT237" s="2">
         <v>31975</v>
       </c>
+      <c r="CU237" s="2">
+        <v>32060</v>
+      </c>
     </row>
-    <row r="238" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>235</v>
       </c>
@@ -72028,8 +72736,11 @@
       <c r="CT238" s="2">
         <v>66497</v>
       </c>
+      <c r="CU238" s="2">
+        <v>66980</v>
+      </c>
     </row>
-    <row r="239" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>236</v>
       </c>
@@ -72324,8 +73035,11 @@
       <c r="CT239" s="2">
         <v>17304</v>
       </c>
+      <c r="CU239" s="2">
+        <v>17559</v>
+      </c>
     </row>
-    <row r="240" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>237</v>
       </c>
@@ -72620,8 +73334,11 @@
       <c r="CT240" s="2">
         <v>3164</v>
       </c>
+      <c r="CU240" s="2">
+        <v>3189</v>
+      </c>
     </row>
-    <row r="241" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>238</v>
       </c>
@@ -72916,8 +73633,11 @@
       <c r="CT241" s="2">
         <v>21597</v>
       </c>
+      <c r="CU241" s="2">
+        <v>22274</v>
+      </c>
     </row>
-    <row r="242" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>239</v>
       </c>
@@ -73212,8 +73932,11 @@
       <c r="CT242" s="2">
         <v>182231</v>
       </c>
+      <c r="CU242" s="2">
+        <v>185145</v>
+      </c>
     </row>
-    <row r="243" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>240</v>
       </c>
@@ -73508,8 +74231,11 @@
       <c r="CT243" s="2">
         <v>20258</v>
       </c>
+      <c r="CU243" s="2">
+        <v>20378</v>
+      </c>
     </row>
-    <row r="244" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>241</v>
       </c>
@@ -73804,8 +74530,11 @@
       <c r="CT244" s="2">
         <v>2561</v>
       </c>
+      <c r="CU244" s="2">
+        <v>2565</v>
+      </c>
     </row>
-    <row r="245" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>242</v>
       </c>
@@ -74100,8 +74829,11 @@
       <c r="CT245" s="2">
         <v>76178</v>
       </c>
+      <c r="CU245" s="2">
+        <v>76972</v>
+      </c>
     </row>
-    <row r="246" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>243</v>
       </c>
@@ -74396,8 +75128,11 @@
       <c r="CT246" s="2">
         <v>9441</v>
       </c>
+      <c r="CU246" s="2">
+        <v>9470</v>
+      </c>
     </row>
-    <row r="247" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>244</v>
       </c>
@@ -74692,8 +75427,11 @@
       <c r="CT247" s="2">
         <v>13909</v>
       </c>
+      <c r="CU247" s="2">
+        <v>14029</v>
+      </c>
     </row>
-    <row r="248" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>245</v>
       </c>
@@ -74988,8 +75726,11 @@
       <c r="CT248" s="2">
         <v>242134</v>
       </c>
+      <c r="CU248" s="2">
+        <v>245596</v>
+      </c>
     </row>
-    <row r="249" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>246</v>
       </c>
@@ -75284,8 +76025,11 @@
       <c r="CT249" s="2">
         <v>17590</v>
       </c>
+      <c r="CU249" s="2">
+        <v>17833</v>
+      </c>
     </row>
-    <row r="250" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>247</v>
       </c>
@@ -75580,8 +76324,11 @@
       <c r="CT250" s="2">
         <v>746</v>
       </c>
+      <c r="CU250" s="2">
+        <v>757</v>
+      </c>
     </row>
-    <row r="251" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>248</v>
       </c>
@@ -75876,8 +76623,11 @@
       <c r="CT251" s="2">
         <v>29729</v>
       </c>
+      <c r="CU251" s="2">
+        <v>29986</v>
+      </c>
     </row>
-    <row r="252" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>249</v>
       </c>
@@ -76172,8 +76922,11 @@
       <c r="CT252" s="2">
         <v>12404</v>
       </c>
+      <c r="CU252" s="2">
+        <v>12546</v>
+      </c>
     </row>
-    <row r="253" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>250</v>
       </c>
@@ -76468,8 +77221,11 @@
       <c r="CT253" s="2">
         <v>2196</v>
       </c>
+      <c r="CU253" s="2">
+        <v>2209</v>
+      </c>
     </row>
-    <row r="254" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>251</v>
       </c>
@@ -76764,8 +77520,11 @@
       <c r="CT254" s="2">
         <v>5437</v>
       </c>
+      <c r="CU254" s="2">
+        <v>5455</v>
+      </c>
     </row>
-    <row r="255" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>252</v>
       </c>
@@ -77060,8 +77819,11 @@
       <c r="CT255" s="2">
         <v>9379</v>
       </c>
+      <c r="CU255" s="2">
+        <v>9389</v>
+      </c>
     </row>
-    <row r="256" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>253</v>
       </c>
@@ -77356,8 +78118,11 @@
       <c r="CT256" s="2">
         <v>5057</v>
       </c>
+      <c r="CU256" s="2">
+        <v>5132</v>
+      </c>
     </row>
-    <row r="257" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>254</v>
       </c>
@@ -77652,8 +78417,11 @@
       <c r="CT257" s="2">
         <v>121100</v>
       </c>
+      <c r="CU257" s="2">
+        <v>121192</v>
+      </c>
     </row>
-    <row r="258" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:99" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>256</v>
       </c>
@@ -77951,8 +78719,11 @@
       <c r="CT258" s="8">
         <v>14189044</v>
       </c>
+      <c r="CU258" s="8">
+        <v>14310667</v>
+      </c>
     </row>
-    <row r="259" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:99" x14ac:dyDescent="0.3">
       <c r="J259" t="s">
         <v>258</v>
       </c>
@@ -77979,7 +78750,7 @@
       <c r="AL259" s="2"/>
       <c r="AM259" s="2"/>
     </row>
-    <row r="260" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M260" s="2"/>
       <c r="P260" s="2"/>
       <c r="Q260" s="2"/>
@@ -77987,7 +78758,7 @@
       <c r="S260" s="2"/>
       <c r="T260" s="2"/>
     </row>
-    <row r="261" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M261" s="2"/>
       <c r="P261" s="2"/>
       <c r="Q261" s="2"/>
@@ -77995,7 +78766,7 @@
       <c r="S261" s="2"/>
       <c r="T261" s="2"/>
     </row>
-    <row r="262" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M262" s="2"/>
       <c r="P262" s="2"/>
       <c r="Q262" s="2"/>
@@ -78003,7 +78774,7 @@
       <c r="S262" s="2"/>
       <c r="T262" s="2"/>
     </row>
-    <row r="263" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M263" s="2"/>
       <c r="P263" s="2"/>
       <c r="Q263" s="2"/>
@@ -78011,7 +78782,7 @@
       <c r="S263" s="2"/>
       <c r="T263" s="2"/>
     </row>
-    <row r="264" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M264" s="2"/>
       <c r="P264" s="2"/>
       <c r="Q264" s="2"/>
@@ -78019,7 +78790,7 @@
       <c r="S264" s="2"/>
       <c r="T264" s="2"/>
     </row>
-    <row r="265" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M265" s="2"/>
       <c r="P265" s="2"/>
       <c r="Q265" s="2"/>
@@ -78027,7 +78798,7 @@
       <c r="S265" s="2"/>
       <c r="T265" s="2"/>
     </row>
-    <row r="266" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M266" s="2"/>
       <c r="P266" s="2"/>
       <c r="Q266" s="2"/>
@@ -78035,7 +78806,7 @@
       <c r="S266" s="2"/>
       <c r="T266" s="2"/>
     </row>
-    <row r="267" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M267" s="2"/>
       <c r="P267" s="2"/>
       <c r="Q267" s="2"/>
@@ -78043,7 +78814,7 @@
       <c r="S267" s="2"/>
       <c r="T267" s="2"/>
     </row>
-    <row r="268" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M268" s="2"/>
       <c r="P268" s="2"/>
       <c r="Q268" s="2"/>
@@ -78051,7 +78822,7 @@
       <c r="S268" s="2"/>
       <c r="T268" s="2"/>
     </row>
-    <row r="269" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M269" s="2"/>
       <c r="P269" s="2"/>
       <c r="Q269" s="2"/>
@@ -78059,7 +78830,7 @@
       <c r="S269" s="2"/>
       <c r="T269" s="2"/>
     </row>
-    <row r="270" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M270" s="2"/>
       <c r="P270" s="2"/>
       <c r="Q270" s="2"/>
@@ -78067,7 +78838,7 @@
       <c r="S270" s="2"/>
       <c r="T270" s="2"/>
     </row>
-    <row r="271" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M271" s="2"/>
       <c r="P271" s="2"/>
       <c r="Q271" s="2"/>
@@ -78075,7 +78846,7 @@
       <c r="S271" s="2"/>
       <c r="T271" s="2"/>
     </row>
-    <row r="272" spans="1:98" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:99" x14ac:dyDescent="0.3">
       <c r="M272" s="2"/>
       <c r="P272" s="2"/>
       <c r="Q272" s="2"/>

</xml_diff>